<commit_message>
added frame for leaderboard
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,18 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>janedoey</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>c78269a8b5134b8f79ae1f2dbb124979effcd3dcad53abf3d4e170b835823847</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>